<commit_message>
Add stats tests for NDVI
</commit_message>
<xml_diff>
--- a/Tests/Validation/NDVI/Lincoln2015RainShelter.xlsx
+++ b/Tests/Validation/NDVI/Lincoln2015RainShelter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\NDVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995B0D54-02F2-4660-8DD2-2BCFA7E8BED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F3FC1-66CF-4D4E-B985-E187FA847D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB7C6092-D139-4796-9226-4E3721A0E685}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{EB7C6092-D139-4796-9226-4E3721A0E685}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -86,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,13 +425,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14A466D-30BF-4DF5-87EE-9DDF5956F927}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,7 +450,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>42286</v>
       </c>
       <c r="C2">
@@ -459,7 +461,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>42289</v>
       </c>
       <c r="C3">
@@ -470,7 +472,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>42292</v>
       </c>
       <c r="C4">
@@ -481,7 +483,7 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>42297</v>
       </c>
       <c r="C5">
@@ -492,7 +494,7 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>42299</v>
       </c>
       <c r="C6">
@@ -503,7 +505,7 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>42304</v>
       </c>
       <c r="C7">
@@ -514,7 +516,7 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>42307</v>
       </c>
       <c r="C8">
@@ -525,7 +527,7 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>42310</v>
       </c>
       <c r="C9">
@@ -536,7 +538,7 @@
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>42313</v>
       </c>
       <c r="C10">
@@ -547,7 +549,7 @@
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>42318</v>
       </c>
       <c r="C11">
@@ -558,7 +560,7 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>42320</v>
       </c>
       <c r="C12">
@@ -569,7 +571,7 @@
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>42325</v>
       </c>
       <c r="C13">
@@ -580,7 +582,7 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>42328</v>
       </c>
       <c r="C14">
@@ -591,7 +593,7 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>42331</v>
       </c>
       <c r="C15">
@@ -602,7 +604,7 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>42338</v>
       </c>
       <c r="C16">
@@ -613,7 +615,7 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>42342</v>
       </c>
       <c r="C17">
@@ -624,7 +626,7 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>42345</v>
       </c>
       <c r="C18">
@@ -635,7 +637,7 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>42349</v>
       </c>
       <c r="C19">
@@ -646,7 +648,7 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>42352</v>
       </c>
       <c r="C20">
@@ -657,7 +659,7 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>42359</v>
       </c>
       <c r="C21">
@@ -668,7 +670,7 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>42368</v>
       </c>
       <c r="C22">
@@ -679,7 +681,7 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>42374</v>
       </c>
       <c r="C23">
@@ -690,7 +692,7 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>42380</v>
       </c>
       <c r="C24">
@@ -701,7 +703,7 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>42383</v>
       </c>
       <c r="C25">
@@ -712,7 +714,7 @@
       <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>42388</v>
       </c>
       <c r="C26">
@@ -723,7 +725,7 @@
       <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>42391</v>
       </c>
       <c r="C27">
@@ -734,7 +736,7 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>42394</v>
       </c>
       <c r="C28">
@@ -745,7 +747,7 @@
       <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>42398</v>
       </c>
       <c r="C29">
@@ -756,7 +758,7 @@
       <c r="A30" t="s">
         <v>2</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>42401</v>
       </c>
       <c r="C30">
@@ -767,7 +769,7 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>42409</v>
       </c>
       <c r="C31">
@@ -778,7 +780,7 @@
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>42286</v>
       </c>
       <c r="C32">
@@ -789,7 +791,7 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>42289</v>
       </c>
       <c r="C33">
@@ -800,7 +802,7 @@
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>42292</v>
       </c>
       <c r="C34">
@@ -811,7 +813,7 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>42297</v>
       </c>
       <c r="C35">
@@ -822,7 +824,7 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>42299</v>
       </c>
       <c r="C36">
@@ -833,7 +835,7 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>42304</v>
       </c>
       <c r="C37">
@@ -844,7 +846,7 @@
       <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>42307</v>
       </c>
       <c r="C38">
@@ -855,7 +857,7 @@
       <c r="A39" t="s">
         <v>3</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>42310</v>
       </c>
       <c r="C39">
@@ -866,7 +868,7 @@
       <c r="A40" t="s">
         <v>3</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>42313</v>
       </c>
       <c r="C40">
@@ -877,7 +879,7 @@
       <c r="A41" t="s">
         <v>3</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>42318</v>
       </c>
       <c r="C41">
@@ -888,7 +890,7 @@
       <c r="A42" t="s">
         <v>3</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>42320</v>
       </c>
       <c r="C42">
@@ -899,7 +901,7 @@
       <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>42325</v>
       </c>
       <c r="C43">
@@ -910,7 +912,7 @@
       <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>42328</v>
       </c>
       <c r="C44">
@@ -921,7 +923,7 @@
       <c r="A45" t="s">
         <v>3</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>42331</v>
       </c>
       <c r="C45">
@@ -932,7 +934,7 @@
       <c r="A46" t="s">
         <v>3</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>42338</v>
       </c>
       <c r="C46">
@@ -943,7 +945,7 @@
       <c r="A47" t="s">
         <v>3</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>42342</v>
       </c>
       <c r="C47">
@@ -954,7 +956,7 @@
       <c r="A48" t="s">
         <v>3</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>42345</v>
       </c>
       <c r="C48">
@@ -965,7 +967,7 @@
       <c r="A49" t="s">
         <v>3</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>42349</v>
       </c>
       <c r="C49">
@@ -976,7 +978,7 @@
       <c r="A50" t="s">
         <v>3</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>42352</v>
       </c>
       <c r="C50">
@@ -987,7 +989,7 @@
       <c r="A51" t="s">
         <v>3</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>42359</v>
       </c>
       <c r="C51">
@@ -998,7 +1000,7 @@
       <c r="A52" t="s">
         <v>3</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>42368</v>
       </c>
       <c r="C52">
@@ -1009,7 +1011,7 @@
       <c r="A53" t="s">
         <v>3</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>42374</v>
       </c>
       <c r="C53">
@@ -1020,7 +1022,7 @@
       <c r="A54" t="s">
         <v>3</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>42380</v>
       </c>
       <c r="C54">
@@ -1031,7 +1033,7 @@
       <c r="A55" t="s">
         <v>3</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>42383</v>
       </c>
       <c r="C55">
@@ -1042,7 +1044,7 @@
       <c r="A56" t="s">
         <v>3</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>42388</v>
       </c>
       <c r="C56">
@@ -1053,7 +1055,7 @@
       <c r="A57" t="s">
         <v>3</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>42391</v>
       </c>
       <c r="C57">
@@ -1064,7 +1066,7 @@
       <c r="A58" t="s">
         <v>3</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>42394</v>
       </c>
       <c r="C58">
@@ -1075,7 +1077,7 @@
       <c r="A59" t="s">
         <v>3</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>42398</v>
       </c>
       <c r="C59">
@@ -1086,7 +1088,7 @@
       <c r="A60" t="s">
         <v>3</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>42401</v>
       </c>
       <c r="C60">
@@ -1097,7 +1099,7 @@
       <c r="A61" t="s">
         <v>3</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>42409</v>
       </c>
       <c r="C61">

</xml_diff>

<commit_message>
Fix test to use correct variable name
</commit_message>
<xml_diff>
--- a/Tests/Validation/NDVI/Lincoln2015RainShelter.xlsx
+++ b/Tests/Validation/NDVI/Lincoln2015RainShelter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\NDVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F3FC1-66CF-4D4E-B985-E187FA847D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8295AD52-075D-4165-842D-DCE852C90826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{EB7C6092-D139-4796-9226-4E3721A0E685}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB7C6092-D139-4796-9226-4E3721A0E685}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>Lincoln2015NDVICheckIrrWet</t>
   </si>
   <si>
-    <t>NDVI.Value</t>
+    <t>Spectral.NDVI</t>
   </si>
 </sst>
 </file>
@@ -426,16 +426,16 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B61"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -457,7 +457,7 @@
         <v>0.17700000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -468,7 +468,7 @@
         <v>0.17177777777777778</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -479,7 +479,7 @@
         <v>0.16732142857142859</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -490,7 +490,7 @@
         <v>0.1792857142857143</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -501,7 +501,7 @@
         <v>0.17517857142857138</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>0.16490243902439028</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -523,7 +523,7 @@
         <v>0.19400000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -534,7 +534,7 @@
         <v>0.14697058823529408</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -545,7 +545,7 @@
         <v>0.15260784313725487</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -556,7 +556,7 @@
         <v>0.13608823529411765</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -567,7 +567,7 @@
         <v>0.13608823529411765</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -578,7 +578,7 @@
         <v>0.13975000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -589,7 +589,7 @@
         <v>0.14927777777777776</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -600,7 +600,7 @@
         <v>0.15170588235294116</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0.13394444444444445</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -622,7 +622,7 @@
         <v>0.13912121212121215</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -633,7 +633,7 @@
         <v>0.13661290322580646</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -644,7 +644,7 @@
         <v>0.12242105263157894</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -655,7 +655,7 @@
         <v>0.15776470588235292</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -666,7 +666,7 @@
         <v>0.1272307692307692</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -677,7 +677,7 @@
         <v>0.12338709677419357</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0.13934782608695648</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -699,7 +699,7 @@
         <v>0.13175000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.12406666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -721,7 +721,7 @@
         <v>0.14729411764705883</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -732,7 +732,7 @@
         <v>0.14737931034482757</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -743,7 +743,7 @@
         <v>0.14527586206896548</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -754,7 +754,7 @@
         <v>0.14527586206896548</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -765,7 +765,7 @@
         <v>0.16966666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -776,7 +776,7 @@
         <v>0.13899999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0.17700000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0.17177777777777778</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0.16732142857142859</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -820,7 +820,7 @@
         <v>0.1792857142857143</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -831,7 +831,7 @@
         <v>0.17517857142857138</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0.16490243902439028</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -853,7 +853,7 @@
         <v>0.2250833333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -864,7 +864,7 @@
         <v>0.26678378378378376</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -875,7 +875,7 @@
         <v>0.24743902439024393</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>0.13608823529411765</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -897,7 +897,7 @@
         <v>0.19321621621621624</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0.13975000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -919,7 +919,7 @@
         <v>0.22747222222222219</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -930,7 +930,7 @@
         <v>0.15170588235294116</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0.13394444444444445</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0.20640740740740746</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -963,7 +963,7 @@
         <v>0.20727586206896556</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -974,7 +974,7 @@
         <v>0.19307142857142856</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -985,7 +985,7 @@
         <v>0.17296296296296293</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -996,7 +996,7 @@
         <v>0.1942105263157895</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>0.12338709677419357</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>0.13934782608695648</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0.19827272727272727</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0.19325925925925927</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>0.17132258064516132</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0.19683333333333333</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0.19917241379310344</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0.14527586206896548</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>0.16966666666666669</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>3</v>
       </c>

</xml_diff>